<commit_message>
Changing the size of a table cell on the third tab of the app
</commit_message>
<xml_diff>
--- a/test/aud_type_85.xlsx
+++ b/test/aud_type_85.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>lesson</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Рус. яз.</t>
+  </si>
+  <si>
+    <t>Спортивные снаряды</t>
   </si>
 </sst>
 </file>
@@ -429,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +462,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>